<commit_message>
Made some icon changes
</commit_message>
<xml_diff>
--- a/backend/slack-hrbp/Attendance_Report_2025-03.xlsx
+++ b/backend/slack-hrbp/Attendance_Report_2025-03.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="31">
   <si>
     <t>User Name</t>
   </si>
@@ -23,7 +23,16 @@
     <t>Mar-03</t>
   </si>
   <si>
+    <t>Mar-04</t>
+  </si>
+  <si>
     <t>Mar-05</t>
+  </si>
+  <si>
+    <t>Mar-06</t>
+  </si>
+  <si>
+    <t>Mar-07</t>
   </si>
   <si>
     <t>Mar-10</t>
@@ -140,7 +149,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -186,497 +195,614 @@
       <c r="M1" t="s" s="0">
         <v>12</v>
       </c>
+      <c r="N1" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s" s="0">
+        <v>15</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F2" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="G2" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H2" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I2" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="J2" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="K2" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="L2" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="M2" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
+      </c>
+      <c r="N2" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="O2" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="P2" t="s" s="0">
+        <v>17</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F3" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="G3" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H3" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I3" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="J3" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="K3" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="L3" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="M3" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
+      </c>
+      <c r="N3" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="O3" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="P3" t="s" s="0">
+        <v>17</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F4" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="G4" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H4" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I4" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="J4" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="K4" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="L4" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="M4" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
+      </c>
+      <c r="N4" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="O4" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="P4" t="s" s="0">
+        <v>17</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E5" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F5" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="G5" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H5" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I5" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="J5" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="K5" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="L5" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="M5" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
+      </c>
+      <c r="N5" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="O5" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="P5" t="s" s="0">
+        <v>17</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E6" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F6" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="G6" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H6" t="s" s="0">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I6" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="J6" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="K6" t="s" s="0">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="L6" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="M6" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
+      </c>
+      <c r="N6" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="O6" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="P6" t="s" s="0">
+        <v>17</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D7" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E7" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F7" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="G7" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H7" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I7" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="J7" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="K7" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="L7" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="M7" t="s" s="0">
-        <v>19</v>
+        <v>17</v>
+      </c>
+      <c r="N7" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="O7" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="P7" t="s" s="0">
+        <v>22</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s" s="0">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D8" t="s" s="0">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="E8" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F8" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="G8" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H8" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I8" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="J8" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="K8" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="L8" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="M8" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
+      </c>
+      <c r="N8" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="O8" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="P8" t="s" s="0">
+        <v>17</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D9" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E9" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F9" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="G9" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H9" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I9" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="J9" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="K9" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="L9" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="M9" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
+      </c>
+      <c r="N9" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="O9" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="P9" t="s" s="0">
+        <v>17</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D10" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E10" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F10" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="G10" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H10" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I10" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="J10" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="K10" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="L10" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="M10" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
+      </c>
+      <c r="N10" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="O10" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="P10" t="s" s="0">
+        <v>17</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C11" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D11" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E11" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F11" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="G11" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H11" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I11" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="J11" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="K11" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="L11" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="M11" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
+      </c>
+      <c r="N11" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="O11" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="P11" t="s" s="0">
+        <v>17</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C12" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D12" t="s" s="0">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E12" t="s" s="0">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="F12" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="G12" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H12" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I12" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="J12" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="K12" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="L12" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="M12" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
+      </c>
+      <c r="N12" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="O12" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="P12" t="s" s="0">
+        <v>17</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C13" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D13" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E13" t="s" s="0">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F13" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="G13" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H13" t="s" s="0">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="I13" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="J13" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="K13" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="L13" t="s" s="0">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="M13" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
+      </c>
+      <c r="N13" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="O13" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="P13" t="s" s="0">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changed to JWT token Everywhere
</commit_message>
<xml_diff>
--- a/backend/slack-hrbp/Attendance_Report_2025-03.xlsx
+++ b/backend/slack-hrbp/Attendance_Report_2025-03.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="38">
   <si>
     <t>User Name</t>
   </si>
@@ -30,9 +30,6 @@
   </si>
   <si>
     <t>Mar-06</t>
-  </si>
-  <si>
-    <t>Mar-07</t>
   </si>
   <si>
     <t>Mar-10</t>
@@ -173,7 +170,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:V13"/>
+  <dimension ref="A1:U13"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -243,824 +240,785 @@
       <c r="U1" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="V1" t="s" s="0">
-        <v>21</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F2" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G2" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H2" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I2" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J2" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K2" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L2" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M2" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N2" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O2" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P2" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q2" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R2" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S2" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="T2" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="U2" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="V2" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F3" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G3" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H3" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I3" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J3" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K3" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L3" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M3" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N3" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O3" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P3" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q3" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R3" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S3" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="T3" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="U3" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="V3" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E4" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F4" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G4" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H4" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I4" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J4" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K4" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L4" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M4" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N4" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O4" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P4" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q4" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R4" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S4" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="T4" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="U4" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="V4" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E5" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F5" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G5" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H5" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I5" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J5" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K5" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L5" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M5" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N5" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O5" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P5" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q5" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R5" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S5" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="T5" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="U5" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="V5" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="E6" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="F6" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="G6" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="H6" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="I6" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="J6" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="K6" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L6" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="M6" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="N6" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="O6" t="s" s="0">
         <v>27</v>
       </c>
-      <c r="B6" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="C6" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="D6" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="E6" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="F6" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="G6" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="H6" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="I6" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="J6" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="K6" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="L6" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="M6" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="N6" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="O6" t="s" s="0">
-        <v>23</v>
-      </c>
       <c r="P6" t="s" s="0">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="Q6" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R6" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S6" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="T6" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="U6" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="V6" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C7" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D7" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E7" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F7" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G7" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H7" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I7" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J7" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K7" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L7" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M7" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N7" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O7" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P7" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q7" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R7" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S7" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="T7" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="U7" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="V7" t="s" s="0">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="E8" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="F8" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="G8" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="B8" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="C8" t="s" s="0">
-        <v>28</v>
-      </c>
-      <c r="D8" t="s" s="0">
-        <v>28</v>
-      </c>
-      <c r="E8" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="F8" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="G8" t="s" s="0">
-        <v>23</v>
-      </c>
       <c r="H8" t="s" s="0">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I8" t="s" s="0">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J8" t="s" s="0">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K8" t="s" s="0">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="L8" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M8" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N8" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O8" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P8" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q8" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R8" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S8" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="T8" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="U8" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="V8" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E9" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F9" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G9" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H9" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I9" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J9" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K9" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L9" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M9" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N9" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O9" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P9" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q9" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R9" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S9" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="T9" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="U9" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="V9" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D10" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E10" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F10" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G10" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H10" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I10" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J10" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K10" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L10" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M10" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N10" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O10" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P10" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q10" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R10" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S10" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="T10" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="U10" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="V10" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C11" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D11" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E11" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F11" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G11" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H11" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I11" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J11" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K11" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L11" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M11" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N11" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O11" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P11" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q11" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R11" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S11" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="T11" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="U11" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="V11" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D12" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E12" t="s" s="0">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F12" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G12" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H12" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I12" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J12" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K12" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L12" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M12" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N12" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O12" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P12" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q12" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R12" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S12" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="T12" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="U12" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="V12" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="0">
+        <v>35</v>
+      </c>
+      <c r="B13" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="E13" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="F13" t="s" s="0">
         <v>36</v>
       </c>
-      <c r="B13" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="C13" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="D13" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="E13" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="F13" t="s" s="0">
+      <c r="G13" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="H13" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="I13" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="J13" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="K13" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="L13" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="M13" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="N13" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="G13" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="H13" t="s" s="0">
-        <v>28</v>
-      </c>
-      <c r="I13" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="J13" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="K13" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="L13" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="M13" t="s" s="0">
-        <v>23</v>
-      </c>
-      <c r="N13" t="s" s="0">
-        <v>28</v>
-      </c>
       <c r="O13" t="s" s="0">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="P13" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="Q13" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R13" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S13" t="s" s="0">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="T13" t="s" s="0">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="U13" t="s" s="0">
-        <v>31</v>
-      </c>
-      <c r="V13" t="s" s="0">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>